<commit_message>
Tested consistency with new variables
</commit_message>
<xml_diff>
--- a/Job_Search_Tracker_Template.xlsx
+++ b/Job_Search_Tracker_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>#</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>www.thisisfake.com</t>
+  </si>
+  <si>
+    <t>Pretend Corp.</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>alexrogers823@yahoo.com</t>
+  </si>
+  <si>
+    <t>www.notimportant.com</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Python</t>
   </si>
 </sst>
 </file>
@@ -449,7 +467,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="H2" xSplit="1" ySplit="1"/>
@@ -575,6 +593,35 @@
         <v>29</v>
       </c>
     </row>
+    <row r="4" spans="1:13">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K2" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed subject title and line breaks in message
</commit_message>
<xml_diff>
--- a/Job_Search_Tracker_Template.xlsx
+++ b/Job_Search_Tracker_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -121,10 +121,55 @@
     <t>www.notimportant.com</t>
   </si>
   <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Bullhorn</t>
+  </si>
+  <si>
+    <t>Junior Software Engineer</t>
+  </si>
+  <si>
+    <t>Aqeelah Jones</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/search/?currentJobId=890579596&amp;keywords=software%20developer&amp;location=Greater%20Atlanta%20Area&amp;locationId=us%3A52</t>
+  </si>
+  <si>
     <t>Open</t>
   </si>
   <si>
-    <t>Python</t>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Infor</t>
+  </si>
+  <si>
+    <t>Allie Persinger</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/search/?currentJobId=889095712&amp;keywords=software%20developer&amp;location=Greater%20Atlanta%20Area&amp;locationId=us%3A52</t>
+  </si>
+  <si>
+    <t>Brooksource</t>
+  </si>
+  <si>
+    <t>Wynne Rosenbleeth</t>
+  </si>
+  <si>
+    <t>470-419-2504</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/search/?currentJobId=888000630&amp;keywords=software%20developer&amp;location=Greater%20Atlanta%20Area&amp;locationId=us%3A52</t>
   </si>
 </sst>
 </file>
@@ -467,7 +512,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="H2" xSplit="1" ySplit="1"/>
@@ -622,6 +667,96 @@
         <v>35</v>
       </c>
     </row>
+    <row r="5" spans="1:13">
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K2" r:id="rId1"/>

</xml_diff>

<commit_message>
Took out active companies specific to Alex
</commit_message>
<xml_diff>
--- a/Job_Search_Tracker_Template.xlsx
+++ b/Job_Search_Tracker_Template.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexrogers823/Documents/DigitalCrafts/Job-search/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="14180" windowWidth="25600" xWindow="0" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Application Tracker" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Application Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" concurrentCalc="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>#</t>
   </si>
@@ -121,7 +131,7 @@
     <t>www.notimportant.com</t>
   </si>
   <si>
-    <t>Closed</t>
+    <t>Open</t>
   </si>
   <si>
     <t>Python</t>
@@ -139,15 +149,9 @@
     <t>""</t>
   </si>
   <si>
-    <t>Ready</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/jobs/search/?currentJobId=890579596&amp;keywords=software%20developer&amp;location=Greater%20Atlanta%20Area&amp;locationId=us%3A52</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>JavaScript</t>
   </si>
   <si>
@@ -166,44 +170,44 @@
     <t>Wynne Rosenbleeth</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/jobs/search/?currentJobId=888000630&amp;keywords=software%20developer&amp;location=Greater%20Atlanta%20Area&amp;locationId=us%3A52</t>
+  </si>
+  <si>
     <t>470-419-2504</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/jobs/search/?currentJobId=888000630&amp;keywords=software%20developer&amp;location=Greater%20Atlanta%20Area&amp;locationId=us%3A52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt formatCode="m/d/yyyy" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <b val="1"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <color rgb="FF0000FF"/>
-      <sz val="10"/>
-      <u val="single"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -225,23 +229,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -507,36 +517,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="H2" xSplit="1" ySplit="1"/>
-      <selection activeCell="B1" pane="topRight" sqref="B1"/>
-      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="M2" pane="bottomRight" sqref="M2"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="14.5" defaultRowHeight="15.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="6.83203125"/>
-    <col customWidth="1" max="2" min="2" width="19.1640625"/>
-    <col customWidth="1" max="3" min="3" width="21"/>
-    <col customWidth="1" max="4" min="4" width="11.5"/>
-    <col customWidth="1" max="5" min="5" width="15.83203125"/>
-    <col customWidth="1" max="6" min="6" width="18.6640625"/>
-    <col customWidth="1" max="7" min="7" width="22.5"/>
-    <col customWidth="1" max="8" min="8" width="18.1640625"/>
-    <col customWidth="1" max="9" min="9" width="51.5"/>
-    <col customWidth="1" max="10" min="10" width="17.33203125"/>
-    <col customWidth="1" max="11" min="11" width="56.33203125"/>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="51.5" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +586,8 @@
         <v>12</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:13">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -590,7 +599,7 @@
       <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="6">
         <v>42856</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -612,7 +621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row customHeight="1" ht="13" r="3" spans="1:13">
+    <row r="3" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -638,7 +647,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -667,7 +676,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>36</v>
       </c>
@@ -683,22 +692,19 @@
       <c r="G5" t="s">
         <v>39</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
         <v>41</v>
       </c>
-      <c r="L5" t="s">
+    </row>
+    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
         <v>42</v>
-      </c>
-      <c r="M5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="B6" t="s">
-        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -707,27 +713,24 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
         <v>39</v>
       </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
       <c r="K6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -736,31 +739,28 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>